<commit_message>
£HFD FY19, 20 results
</commit_message>
<xml_diff>
--- a/£HFD.xlsx
+++ b/£HFD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E771028E-885C-FD45-8F48-ACA4C4193F12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE1A598-BEAE-7040-847D-B0A4BF90A1FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="18820" activeTab="1" xr2:uid="{3483339E-0186-4DD8-B843-20C8BDA2099F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="109">
   <si>
     <t>£HLF</t>
   </si>
@@ -360,6 +360,9 @@
   </si>
   <si>
     <t>Cashflow Statement</t>
+  </si>
+  <si>
+    <t>FY17</t>
   </si>
 </sst>
 </file>
@@ -368,7 +371,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
-    <numFmt numFmtId="168" formatCode="0.0\x"/>
+    <numFmt numFmtId="165" formatCode="0.0\x"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -566,7 +569,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -596,33 +599,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -653,16 +630,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="17" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -678,6 +646,46 @@
     <xf numFmtId="14" fontId="7" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -766,15 +774,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>23</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>100</xdr:row>
+      <xdr:row>105</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -824,7 +832,7 @@
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>100</xdr:row>
+      <xdr:row>105</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1167,7 +1175,7 @@
   <dimension ref="B2:O39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="N41" sqref="N41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1179,14 +1187,14 @@
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="46" t="s">
+      <c r="F2" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B3" s="2" t="s">
@@ -1194,22 +1202,22 @@
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="21"/>
-      <c r="G5" s="19" t="s">
+      <c r="C5" s="43"/>
+      <c r="D5" s="44"/>
+      <c r="G5" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="21"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="43"/>
+      <c r="L5" s="43"/>
+      <c r="M5" s="43"/>
+      <c r="N5" s="43"/>
+      <c r="O5" s="44"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B6" s="3" t="s">
@@ -1233,7 +1241,7 @@
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="28">
+      <c r="C7" s="18">
         <v>205.7</v>
       </c>
       <c r="D7" s="15" t="str">
@@ -1254,7 +1262,7 @@
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="28">
+      <c r="C8" s="18">
         <f>C6*C7</f>
         <v>357.91800000000001</v>
       </c>
@@ -1273,8 +1281,8 @@
       <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="28">
-        <f>'Financial Model'!W62</f>
+      <c r="C9" s="18">
+        <f>'Financial Model'!X62</f>
         <v>50.5</v>
       </c>
       <c r="D9" s="15" t="str">
@@ -1295,8 +1303,8 @@
       <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="28">
-        <f>'Financial Model'!W63</f>
+      <c r="C10" s="18">
+        <f>'Financial Model'!X63</f>
         <v>0.7</v>
       </c>
       <c r="D10" s="15" t="str">
@@ -1317,7 +1325,7 @@
       <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="28">
+      <c r="C11" s="18">
         <f>C9-C10</f>
         <v>49.8</v>
       </c>
@@ -1339,7 +1347,7 @@
       <c r="B12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="29">
+      <c r="C12" s="19">
         <f>C8-C11</f>
         <v>308.11799999999999</v>
       </c>
@@ -1377,11 +1385,11 @@
       <c r="O14" s="7"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="21"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="44"/>
       <c r="G15" s="13"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
@@ -1396,10 +1404,10 @@
       <c r="B16" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="23"/>
+      <c r="D16" s="41"/>
       <c r="G16" s="13"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
@@ -1414,10 +1422,10 @@
       <c r="B17" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="23"/>
+      <c r="D17" s="41"/>
       <c r="G17" s="13"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
@@ -1432,10 +1440,10 @@
       <c r="B18" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="23"/>
+      <c r="D18" s="41"/>
       <c r="G18" s="13"/>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
@@ -1450,10 +1458,10 @@
       <c r="B19" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="24" t="s">
+      <c r="C19" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="25"/>
+      <c r="D19" s="46"/>
       <c r="G19" s="14"/>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
@@ -1465,70 +1473,70 @@
       <c r="O19" s="10"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="21"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="44"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B23" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="22" t="s">
+      <c r="C23" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="23"/>
+      <c r="D23" s="41"/>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B24" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="22">
+      <c r="C24" s="40">
         <v>1892</v>
       </c>
-      <c r="D24" s="23"/>
+      <c r="D24" s="41"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B25" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="22">
+      <c r="C25" s="40">
         <v>2004</v>
       </c>
-      <c r="D25" s="23"/>
+      <c r="D25" s="41"/>
       <c r="E25" s="1" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B26" s="11"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="23"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="41"/>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B27" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="22">
-        <f>'Financial Model'!W33</f>
+      <c r="C27" s="40">
+        <f>'Financial Model'!X33</f>
         <v>222.1</v>
       </c>
-      <c r="D27" s="23"/>
+      <c r="D27" s="41"/>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B28" s="11"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="23"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="41"/>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B29" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="42" t="s">
+      <c r="C29" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="D29" s="43">
+      <c r="D29" s="32">
         <v>44713</v>
       </c>
     </row>
@@ -1536,84 +1544,77 @@
       <c r="B30" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="26" t="s">
+      <c r="C30" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="D30" s="27"/>
+      <c r="D30" s="52"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B33" s="19" t="s">
+      <c r="B33" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="C33" s="20"/>
-      <c r="D33" s="21"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="44"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B34" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C34" s="44">
-        <f>C6/'Financial Model'!W60</f>
+      <c r="C34" s="47">
+        <f>C6/'Financial Model'!X60</f>
         <v>0.64957894736842103</v>
       </c>
-      <c r="D34" s="45"/>
+      <c r="D34" s="48"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B35" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C35" s="44">
-        <f>C8/'Financial Model'!W4</f>
+      <c r="C35" s="47">
+        <f>C8/'Financial Model'!X4</f>
         <v>0.26133031542056079</v>
       </c>
-      <c r="D35" s="45"/>
+      <c r="D35" s="48"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B36" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="44">
-        <f>C12/'Financial Model'!W4</f>
+      <c r="C36" s="47">
+        <f>C12/'Financial Model'!X4</f>
         <v>0.22496933411214953</v>
       </c>
-      <c r="D36" s="45"/>
+      <c r="D36" s="48"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B37" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C37" s="44">
-        <f>C6/'Financial Model'!W13</f>
+      <c r="C37" s="47">
+        <f>C6/'Financial Model'!X13</f>
         <v>4.6064092664092673</v>
       </c>
-      <c r="D37" s="45"/>
+      <c r="D37" s="48"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B38" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C38" s="44">
-        <f>C12/'Financial Model'!W12</f>
+      <c r="C38" s="47">
+        <f>C12/'Financial Model'!X12</f>
         <v>3.9654826254826259</v>
       </c>
-      <c r="D38" s="45"/>
+      <c r="D38" s="48"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B39" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="C39" s="17"/>
-      <c r="D39" s="18"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="C37:D37"/>
     <mergeCell ref="C38:D38"/>
@@ -1629,6 +1630,13 @@
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C30:D30" r:id="rId1" display="Link" xr:uid="{07676FE1-E26A-AE4D-A21B-792EB2B848FD}"/>
@@ -1641,13 +1649,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFF52FD5-5387-455B-8CDC-129D27EFA8D5}">
-  <dimension ref="B1:AF74"/>
+  <dimension ref="B1:AG79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="D27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomRight" activeCell="X76" sqref="A76:XFD76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1655,901 +1663,1459 @@
     <col min="1" max="1" width="4.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="28.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.1640625" style="50"/>
+    <col min="4" max="4" width="9.1640625" style="37"/>
     <col min="5" max="5" width="9.1640625" style="1"/>
-    <col min="6" max="6" width="9.1640625" style="50"/>
+    <col min="6" max="6" width="9.1640625" style="37"/>
     <col min="7" max="7" width="9.1640625" style="1"/>
-    <col min="8" max="8" width="9.1640625" style="50"/>
+    <col min="8" max="8" width="9.1640625" style="37"/>
     <col min="9" max="9" width="9.1640625" style="1"/>
-    <col min="10" max="10" width="9.1640625" style="50"/>
+    <col min="10" max="10" width="9.1640625" style="37"/>
     <col min="11" max="11" width="9.1640625" style="1"/>
-    <col min="12" max="12" width="9.1640625" style="50"/>
+    <col min="12" max="12" width="9.1640625" style="37"/>
     <col min="13" max="13" width="9.1640625" style="1"/>
-    <col min="14" max="14" width="9.1640625" style="50"/>
+    <col min="14" max="14" width="9.1640625" style="37"/>
     <col min="15" max="15" width="9.1640625" style="1"/>
-    <col min="16" max="16" width="9.1640625" style="50"/>
+    <col min="16" max="16" width="9.1640625" style="37"/>
     <col min="17" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:32" s="31" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="C1" s="31" t="s">
+    <row r="1" spans="2:33" s="21" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="C1" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="47" t="s">
+      <c r="F1" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="47" t="s">
+      <c r="H1" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="I1" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="47" t="s">
+      <c r="J1" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="K1" s="31" t="s">
+      <c r="K1" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="L1" s="47" t="s">
+      <c r="L1" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="M1" s="31" t="s">
+      <c r="M1" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="N1" s="47" t="s">
+      <c r="N1" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="O1" s="31" t="s">
+      <c r="O1" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="P1" s="47" t="s">
+      <c r="P1" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="S1" s="31" t="s">
+      <c r="S1" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="T1" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="T1" s="31" t="s">
+      <c r="U1" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="U1" s="31" t="s">
+      <c r="V1" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="V1" s="31" t="s">
+      <c r="W1" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="W1" s="36" t="s">
+      <c r="X1" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="X1" s="31" t="s">
+      <c r="Y1" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="Y1" s="31" t="s">
+      <c r="Z1" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="Z1" s="31" t="s">
+      <c r="AA1" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="AA1" s="31" t="s">
+      <c r="AB1" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="AB1" s="31" t="s">
+      <c r="AC1" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="AC1" s="31" t="s">
+      <c r="AD1" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="AD1" s="31" t="s">
+      <c r="AE1" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="AE1" s="31" t="s">
+      <c r="AF1" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="AF1" s="31" t="s">
+      <c r="AG1" s="21" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="2:32" s="33" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="32"/>
-      <c r="D2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="35">
+    <row r="2" spans="2:33" s="23" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B2" s="22"/>
+      <c r="D2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="25">
         <v>44106</v>
       </c>
-      <c r="J2" s="52">
+      <c r="J2" s="39">
         <v>44288</v>
       </c>
-      <c r="K2" s="35">
+      <c r="K2" s="25">
         <v>44470</v>
       </c>
-      <c r="L2" s="48"/>
-      <c r="N2" s="48"/>
-      <c r="P2" s="48"/>
-      <c r="V2" s="35">
+      <c r="L2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="U2" s="25">
+        <v>43553</v>
+      </c>
+      <c r="V2" s="25">
+        <v>43924</v>
+      </c>
+      <c r="W2" s="25">
         <v>44288</v>
       </c>
-      <c r="W2" s="35">
+      <c r="X2" s="25">
         <v>44652</v>
       </c>
     </row>
-    <row r="3" spans="2:32" s="33" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="32"/>
-      <c r="D3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="34">
+    <row r="3" spans="2:33" s="23" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B3" s="22"/>
+      <c r="D3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="24">
         <v>44510</v>
       </c>
-      <c r="L3" s="48"/>
-      <c r="M3" s="34">
+      <c r="L3" s="35"/>
+      <c r="M3" s="24">
         <v>44868</v>
       </c>
-      <c r="N3" s="48"/>
-      <c r="P3" s="48"/>
-      <c r="W3" s="34">
+      <c r="N3" s="35"/>
+      <c r="P3" s="35"/>
+      <c r="V3" s="24"/>
+      <c r="X3" s="24">
         <v>44728</v>
       </c>
     </row>
-    <row r="4" spans="2:32" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:33" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B4" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="H4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="L4" s="49"/>
-      <c r="N4" s="49"/>
-      <c r="P4" s="49"/>
-      <c r="V4" s="37">
+      <c r="D4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="L4" s="36"/>
+      <c r="N4" s="36"/>
+      <c r="P4" s="36"/>
+      <c r="U4" s="27">
+        <v>1138.5999999999999</v>
+      </c>
+      <c r="V4" s="27">
+        <v>1155.0999999999999</v>
+      </c>
+      <c r="W4" s="27">
         <v>1292.3</v>
       </c>
-      <c r="W4" s="37">
+      <c r="X4" s="27">
         <v>1369.6</v>
       </c>
     </row>
-    <row r="5" spans="2:32" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:33" x14ac:dyDescent="0.15">
       <c r="B5" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="V5" s="28">
+      <c r="U5" s="18">
+        <v>559.6</v>
+      </c>
+      <c r="V5" s="18">
+        <v>565.4</v>
+      </c>
+      <c r="W5" s="18">
         <v>636</v>
       </c>
-      <c r="W5" s="28">
+      <c r="X5" s="18">
         <v>647.9</v>
       </c>
     </row>
-    <row r="6" spans="2:32" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:33" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B6" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="H6" s="49"/>
-      <c r="J6" s="49"/>
-      <c r="L6" s="49"/>
-      <c r="N6" s="49"/>
-      <c r="P6" s="49"/>
-      <c r="V6" s="37">
+      <c r="D6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="J6" s="36"/>
+      <c r="L6" s="36"/>
+      <c r="N6" s="36"/>
+      <c r="P6" s="36"/>
+      <c r="U6" s="27">
+        <f>U4-U5</f>
+        <v>578.99999999999989</v>
+      </c>
+      <c r="V6" s="27">
         <f>V4-V5</f>
+        <v>589.69999999999993</v>
+      </c>
+      <c r="W6" s="27">
+        <f>W4-W5</f>
         <v>656.3</v>
       </c>
-      <c r="W6" s="37">
-        <f>W4-W5</f>
+      <c r="X6" s="27">
+        <f>X4-X5</f>
         <v>721.69999999999993</v>
       </c>
     </row>
-    <row r="7" spans="2:32" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:33" x14ac:dyDescent="0.15">
       <c r="B7" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="V7" s="28">
+      <c r="U7" s="18">
+        <v>524.6</v>
+      </c>
+      <c r="V7" s="18">
+        <v>556.70000000000005</v>
+      </c>
+      <c r="W7" s="18">
         <v>576.79999999999995</v>
       </c>
-      <c r="W7" s="28">
+      <c r="X7" s="18">
         <v>613.79999999999995</v>
       </c>
     </row>
-    <row r="8" spans="2:32" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:33" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B8" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D8" s="49"/>
-      <c r="F8" s="49"/>
-      <c r="H8" s="49"/>
-      <c r="J8" s="49"/>
-      <c r="L8" s="49"/>
-      <c r="N8" s="49"/>
-      <c r="P8" s="49"/>
-      <c r="V8" s="37">
+      <c r="D8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="J8" s="36"/>
+      <c r="L8" s="36"/>
+      <c r="N8" s="36"/>
+      <c r="P8" s="36"/>
+      <c r="U8" s="27">
+        <f>U6-U7</f>
+        <v>54.399999999999864</v>
+      </c>
+      <c r="V8" s="27">
         <f>V6-V7</f>
+        <v>32.999999999999886</v>
+      </c>
+      <c r="W8" s="27">
+        <f>W6-W7</f>
         <v>79.5</v>
       </c>
-      <c r="W8" s="37">
-        <f>W6-W7</f>
+      <c r="X8" s="27">
+        <f>X6-X7</f>
         <v>107.89999999999998</v>
       </c>
     </row>
-    <row r="9" spans="2:32" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:33" x14ac:dyDescent="0.15">
       <c r="B9" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="V9" s="28">
+      <c r="U9" s="18">
+        <v>3.4</v>
+      </c>
+      <c r="V9" s="18">
+        <f>13.9-0.3</f>
+        <v>13.6</v>
+      </c>
+      <c r="W9" s="18">
         <v>15</v>
       </c>
-      <c r="W9" s="28">
+      <c r="X9" s="18">
         <v>11.3</v>
       </c>
     </row>
-    <row r="10" spans="2:32" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:33" x14ac:dyDescent="0.15">
       <c r="B10" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="V10" s="28">
+      <c r="U10" s="18">
+        <f>U8-U9</f>
+        <v>50.999999999999865</v>
+      </c>
+      <c r="V10" s="18">
         <f>V8-V9</f>
+        <v>19.399999999999885</v>
+      </c>
+      <c r="W10" s="18">
+        <f>W8-W9</f>
         <v>64.5</v>
       </c>
-      <c r="W10" s="28">
-        <f>W8-W9</f>
+      <c r="X10" s="18">
+        <f>X8-X9</f>
         <v>96.59999999999998</v>
       </c>
     </row>
-    <row r="11" spans="2:32" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:33" x14ac:dyDescent="0.15">
       <c r="B11" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="V11" s="28">
+      <c r="U11" s="18">
+        <v>9.1</v>
+      </c>
+      <c r="V11" s="18">
+        <v>1.9</v>
+      </c>
+      <c r="W11" s="18">
         <v>11.3</v>
       </c>
-      <c r="W11" s="28">
+      <c r="X11" s="18">
         <v>18.899999999999999</v>
       </c>
     </row>
-    <row r="12" spans="2:32" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:33" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B12" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D12" s="49"/>
-      <c r="F12" s="49"/>
-      <c r="H12" s="49"/>
-      <c r="J12" s="49"/>
-      <c r="L12" s="49"/>
-      <c r="N12" s="49"/>
-      <c r="P12" s="49"/>
-      <c r="V12" s="37">
+      <c r="D12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="J12" s="36"/>
+      <c r="L12" s="36"/>
+      <c r="N12" s="36"/>
+      <c r="P12" s="36"/>
+      <c r="U12" s="27">
+        <f>U10-U11</f>
+        <v>41.899999999999864</v>
+      </c>
+      <c r="V12" s="27">
         <f>V10-V11</f>
+        <v>17.499999999999886</v>
+      </c>
+      <c r="W12" s="27">
+        <f>W10-W11</f>
         <v>53.2</v>
       </c>
-      <c r="W12" s="37">
-        <f>W10-W11</f>
+      <c r="X12" s="27">
+        <f>X10-X11</f>
         <v>77.699999999999989</v>
       </c>
     </row>
-    <row r="13" spans="2:32" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:33" x14ac:dyDescent="0.15">
       <c r="B13" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="V13" s="38">
+      <c r="U13" s="28">
+        <f>U12/U14</f>
+        <v>0.21044701155198325</v>
+      </c>
+      <c r="V13" s="28">
         <f>V12/V14</f>
+        <v>8.7895529884479587E-2</v>
+      </c>
+      <c r="W13" s="28">
+        <f>W12/W14</f>
         <v>0.26720241084881974</v>
       </c>
-      <c r="W13" s="38">
-        <f>W12/W14</f>
+      <c r="X13" s="28">
+        <f>X12/X14</f>
         <v>0.37773456490034024</v>
       </c>
     </row>
-    <row r="14" spans="2:32" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:33" x14ac:dyDescent="0.15">
       <c r="B14" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="U14" s="1">
+        <v>199.1</v>
+      </c>
       <c r="V14" s="1">
         <v>199.1</v>
       </c>
-      <c r="W14" s="28">
+      <c r="W14" s="1">
+        <v>199.1</v>
+      </c>
+      <c r="X14" s="18">
         <v>205.7</v>
       </c>
     </row>
-    <row r="16" spans="2:32" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="2:33" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B16" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D16" s="49"/>
-      <c r="F16" s="49"/>
-      <c r="H16" s="49"/>
-      <c r="J16" s="49"/>
-      <c r="L16" s="49"/>
-      <c r="N16" s="49"/>
-      <c r="P16" s="49"/>
-      <c r="W16" s="39">
+      <c r="D16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="J16" s="36"/>
+      <c r="L16" s="36"/>
+      <c r="N16" s="36"/>
+      <c r="P16" s="36"/>
+      <c r="V16" s="29">
+        <f>V4/U4-1</f>
+        <v>1.4491480765852716E-2</v>
+      </c>
+      <c r="W16" s="29">
         <f>W4/V4-1</f>
+        <v>0.11877759501341889</v>
+      </c>
+      <c r="X16" s="29">
+        <f>X4/W4-1</f>
         <v>5.9815832237096522E-2</v>
       </c>
     </row>
-    <row r="17" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B17" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="S17" s="30" t="s">
+      <c r="T17" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="T17" s="30" t="s">
+      <c r="U17" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="U17" s="30" t="s">
+      <c r="V17" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="V17" s="30" t="s">
+      <c r="W17" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="W17" s="30" t="s">
+      <c r="X17" s="20" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B19" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="V19" s="40">
-        <f t="shared" ref="V19:W19" si="0">V6/V4</f>
+      <c r="U19" s="30">
+        <f t="shared" ref="U19:V19" si="0">U6/U4</f>
+        <v>0.50851923414719824</v>
+      </c>
+      <c r="V19" s="30">
+        <f t="shared" ref="V19:W19" si="1">V6/V4</f>
+        <v>0.51051856982079469</v>
+      </c>
+      <c r="W19" s="30">
+        <f t="shared" si="1"/>
         <v>0.50785421341793702</v>
       </c>
-      <c r="W19" s="40">
-        <f>W6/W4</f>
+      <c r="X19" s="30">
+        <f>X6/X4</f>
         <v>0.52694217289719625</v>
       </c>
     </row>
-    <row r="20" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B20" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="V20" s="40">
-        <f t="shared" ref="V20:W20" si="1">V8/V4</f>
+      <c r="U20" s="30">
+        <f t="shared" ref="U20:V20" si="2">U8/U4</f>
+        <v>4.7777972949235789E-2</v>
+      </c>
+      <c r="V20" s="30">
+        <f t="shared" ref="V20:W20" si="3">V8/V4</f>
+        <v>2.8568955068825112E-2</v>
+      </c>
+      <c r="W20" s="30">
+        <f t="shared" si="3"/>
         <v>6.1518223322757873E-2</v>
       </c>
-      <c r="W20" s="40">
-        <f>W8/W4</f>
+      <c r="X20" s="30">
+        <f>X8/X4</f>
         <v>7.878212616822429E-2</v>
       </c>
     </row>
-    <row r="21" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B21" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="V21" s="40">
-        <f t="shared" ref="V21:W21" si="2">V12/V4</f>
+      <c r="U21" s="30">
+        <f t="shared" ref="U21:V21" si="4">U12/U4</f>
+        <v>3.6799578429650329E-2</v>
+      </c>
+      <c r="V21" s="30">
+        <f t="shared" ref="V21:W21" si="5">V12/V4</f>
+        <v>1.5150203445589028E-2</v>
+      </c>
+      <c r="W21" s="30">
+        <f t="shared" si="5"/>
         <v>4.1166911707807785E-2</v>
       </c>
-      <c r="W21" s="40">
-        <f>W12/W4</f>
+      <c r="X21" s="30">
+        <f>X12/X4</f>
         <v>5.6731892523364483E-2</v>
       </c>
     </row>
-    <row r="22" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B22" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="V22" s="40">
-        <f t="shared" ref="V22:W22" si="3">V11/V10</f>
+      <c r="U22" s="30">
+        <f t="shared" ref="U22:V22" si="6">U11/U10</f>
+        <v>0.17843137254902008</v>
+      </c>
+      <c r="V22" s="30">
+        <f t="shared" ref="V22:W22" si="7">V11/V10</f>
+        <v>9.7938144329897489E-2</v>
+      </c>
+      <c r="W22" s="30">
+        <f t="shared" si="7"/>
         <v>0.17519379844961241</v>
       </c>
-      <c r="W22" s="40">
-        <f>W11/W10</f>
+      <c r="X22" s="30">
+        <f>X11/X10</f>
         <v>0.19565217391304351</v>
       </c>
     </row>
-    <row r="26" spans="2:23" x14ac:dyDescent="0.15">
-      <c r="B26" s="41" t="s">
+    <row r="26" spans="2:24" x14ac:dyDescent="0.15">
+      <c r="B26" s="31" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B27" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="V27" s="28">
+      <c r="U27" s="18">
+        <v>387.4</v>
+      </c>
+      <c r="V27" s="18">
+        <v>395.7</v>
+      </c>
+      <c r="W27" s="18">
         <v>398.3</v>
       </c>
-      <c r="W27" s="28">
+      <c r="X27" s="18">
         <v>442.4</v>
       </c>
     </row>
-    <row r="28" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B28" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="V28" s="28">
+      <c r="U28" s="18">
+        <v>97.3</v>
+      </c>
+      <c r="V28" s="18">
+        <v>83.1</v>
+      </c>
+      <c r="W28" s="18">
         <v>81.3</v>
       </c>
-      <c r="W28" s="28">
+      <c r="X28" s="18">
         <v>101.7</v>
       </c>
     </row>
-    <row r="29" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="29" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B29" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="V29" s="28">
+      <c r="U29" s="18">
+        <v>0</v>
+      </c>
+      <c r="V29" s="18">
+        <v>349.9</v>
+      </c>
+      <c r="W29" s="18">
         <v>282.8</v>
       </c>
-      <c r="W29" s="28">
+      <c r="X29" s="18">
         <v>350.2</v>
       </c>
     </row>
-    <row r="30" spans="2:23" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="2:24" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B30" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D30" s="49"/>
-      <c r="F30" s="49"/>
-      <c r="H30" s="49"/>
-      <c r="J30" s="49"/>
-      <c r="L30" s="49"/>
-      <c r="N30" s="49"/>
-      <c r="P30" s="49"/>
-      <c r="V30" s="37">
+      <c r="D30" s="36"/>
+      <c r="F30" s="36"/>
+      <c r="H30" s="36"/>
+      <c r="J30" s="36"/>
+      <c r="L30" s="36"/>
+      <c r="N30" s="36"/>
+      <c r="P30" s="36"/>
+      <c r="U30" s="27">
+        <v>0</v>
+      </c>
+      <c r="V30" s="27">
+        <v>0</v>
+      </c>
+      <c r="W30" s="27">
         <v>0.1</v>
       </c>
-      <c r="W30" s="37">
+      <c r="X30" s="27">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="31" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B31" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="V31" s="28">
+      <c r="U31" s="18">
+        <v>0</v>
+      </c>
+      <c r="V31" s="18">
+        <v>7.3</v>
+      </c>
+      <c r="W31" s="18">
         <v>12.3</v>
       </c>
-      <c r="W31" s="28">
+      <c r="X31" s="18">
         <v>14.7</v>
       </c>
     </row>
-    <row r="32" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="32" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B32" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="V32" s="28">
-        <f t="shared" ref="V32" si="4">SUM(V27:V31)</f>
+      <c r="U32" s="18">
+        <f t="shared" ref="U32:W32" si="8">SUM(U27:U31)</f>
+        <v>484.7</v>
+      </c>
+      <c r="V32" s="18">
+        <f t="shared" si="8"/>
+        <v>835.99999999999989</v>
+      </c>
+      <c r="W32" s="18">
+        <f t="shared" si="8"/>
         <v>774.80000000000007</v>
       </c>
-      <c r="W32" s="28">
-        <f>SUM(W27:W31)</f>
+      <c r="X32" s="18">
+        <f>SUM(X27:X31)</f>
         <v>909</v>
       </c>
     </row>
-    <row r="33" spans="2:23" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="2:24" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B33" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D33" s="49"/>
-      <c r="F33" s="49"/>
-      <c r="H33" s="49"/>
-      <c r="J33" s="49"/>
-      <c r="L33" s="49"/>
-      <c r="N33" s="49"/>
-      <c r="P33" s="49"/>
-      <c r="V33" s="37">
+      <c r="D33" s="36"/>
+      <c r="F33" s="36"/>
+      <c r="H33" s="36"/>
+      <c r="J33" s="36"/>
+      <c r="L33" s="36"/>
+      <c r="N33" s="36"/>
+      <c r="P33" s="36"/>
+      <c r="U33" s="27">
+        <v>173.7</v>
+      </c>
+      <c r="V33" s="27">
+        <v>173</v>
+      </c>
+      <c r="W33" s="27">
         <v>143.9</v>
       </c>
-      <c r="W33" s="37">
+      <c r="X33" s="27">
         <v>222.1</v>
       </c>
     </row>
-    <row r="34" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="34" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B34" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="V34" s="28">
+      <c r="U34" s="18">
+        <v>59.1</v>
+      </c>
+      <c r="V34" s="18">
+        <v>53.5</v>
+      </c>
+      <c r="W34" s="18">
         <v>74.099999999999994</v>
       </c>
-      <c r="W34" s="28">
+      <c r="X34" s="18">
         <v>92.6</v>
       </c>
     </row>
-    <row r="35" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="35" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B35" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="V35" s="28">
+      <c r="U35" s="18">
+        <v>0</v>
+      </c>
+      <c r="V35" s="18">
+        <v>0</v>
+      </c>
+      <c r="W35" s="18">
         <v>6</v>
       </c>
-      <c r="W35" s="28">
+      <c r="X35" s="18">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:23" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="2:24" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B36" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D36" s="49"/>
-      <c r="F36" s="49"/>
-      <c r="H36" s="49"/>
-      <c r="J36" s="49"/>
-      <c r="L36" s="49"/>
-      <c r="N36" s="49"/>
-      <c r="P36" s="49"/>
-      <c r="V36" s="37">
+      <c r="D36" s="36"/>
+      <c r="F36" s="36"/>
+      <c r="H36" s="36"/>
+      <c r="J36" s="36"/>
+      <c r="L36" s="36"/>
+      <c r="N36" s="36"/>
+      <c r="P36" s="36"/>
+      <c r="U36" s="27">
+        <v>3.2</v>
+      </c>
+      <c r="V36" s="27">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="W36" s="27">
         <v>0.5</v>
       </c>
-      <c r="W36" s="37">
+      <c r="X36" s="27">
         <v>4.2</v>
       </c>
     </row>
-    <row r="37" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="37" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B37" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="V37" s="28">
+      <c r="U37" s="18">
+        <v>0</v>
+      </c>
+      <c r="V37" s="18">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="W37" s="18">
         <v>3.1</v>
       </c>
-      <c r="W37" s="28">
+      <c r="X37" s="18">
         <v>3.9</v>
       </c>
     </row>
-    <row r="38" spans="2:23" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="2:24" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B38" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D38" s="49"/>
-      <c r="F38" s="49"/>
-      <c r="H38" s="49"/>
-      <c r="J38" s="49"/>
-      <c r="L38" s="49"/>
-      <c r="N38" s="49"/>
-      <c r="P38" s="49"/>
-      <c r="V38" s="37">
+      <c r="D38" s="36"/>
+      <c r="F38" s="36"/>
+      <c r="H38" s="36"/>
+      <c r="J38" s="36"/>
+      <c r="L38" s="36"/>
+      <c r="N38" s="36"/>
+      <c r="P38" s="36"/>
+      <c r="U38" s="27">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="V38" s="27">
+        <v>115.5</v>
+      </c>
+      <c r="W38" s="27">
         <v>67.2</v>
       </c>
-      <c r="W38" s="37">
+      <c r="X38" s="27">
         <v>46.3</v>
       </c>
     </row>
-    <row r="39" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="39" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B39" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="V39" s="28">
-        <f t="shared" ref="V39" si="5">SUM(V32:V38)</f>
+      <c r="U39" s="18">
+        <f t="shared" ref="U39:W39" si="9">SUM(U32:U38)</f>
+        <v>730.5</v>
+      </c>
+      <c r="V39" s="18">
+        <f t="shared" si="9"/>
+        <v>1194.9000000000001</v>
+      </c>
+      <c r="W39" s="18">
+        <f t="shared" si="9"/>
         <v>1069.6000000000001</v>
       </c>
-      <c r="W39" s="28">
-        <f>SUM(W32:W38)</f>
+      <c r="X39" s="18">
+        <f>SUM(X32:X38)</f>
         <v>1278.0999999999999</v>
       </c>
     </row>
-    <row r="40" spans="2:23" x14ac:dyDescent="0.15">
-      <c r="V40" s="28"/>
-    </row>
-    <row r="41" spans="2:23" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="2:24" x14ac:dyDescent="0.15">
+      <c r="W40" s="18"/>
+    </row>
+    <row r="41" spans="2:24" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B41" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D41" s="49"/>
-      <c r="F41" s="49"/>
-      <c r="H41" s="49"/>
-      <c r="J41" s="49"/>
-      <c r="L41" s="49"/>
-      <c r="N41" s="49"/>
-      <c r="P41" s="49"/>
-      <c r="V41" s="37">
+      <c r="D41" s="36"/>
+      <c r="F41" s="36"/>
+      <c r="H41" s="36"/>
+      <c r="J41" s="36"/>
+      <c r="L41" s="36"/>
+      <c r="N41" s="36"/>
+      <c r="P41" s="36"/>
+      <c r="U41" s="2">
+        <v>18.5</v>
+      </c>
+      <c r="V41" s="27">
         <v>0.2</v>
       </c>
-      <c r="W41" s="37">
+      <c r="W41" s="27">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="42" spans="2:23" x14ac:dyDescent="0.15">
+      <c r="X41" s="27">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="42" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B42" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="V42" s="28">
+      <c r="U42" s="1">
+        <v>0</v>
+      </c>
+      <c r="V42" s="18">
+        <v>83.2</v>
+      </c>
+      <c r="W42" s="18">
         <v>63.4</v>
       </c>
-      <c r="W42" s="28">
+      <c r="X42" s="18">
         <v>74.5</v>
       </c>
     </row>
-    <row r="43" spans="2:23" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="2:24" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B43" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D43" s="49"/>
-      <c r="F43" s="49"/>
-      <c r="H43" s="49"/>
-      <c r="J43" s="49"/>
-      <c r="L43" s="49"/>
-      <c r="N43" s="49"/>
-      <c r="P43" s="49"/>
-      <c r="V43" s="37">
+      <c r="D43" s="36"/>
+      <c r="F43" s="36"/>
+      <c r="H43" s="36"/>
+      <c r="J43" s="36"/>
+      <c r="L43" s="36"/>
+      <c r="N43" s="36"/>
+      <c r="P43" s="36"/>
+      <c r="U43" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="V43" s="27">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="W43" s="27">
         <v>5.9</v>
       </c>
-      <c r="W43" s="37">
+      <c r="X43" s="27">
         <v>0.5</v>
       </c>
     </row>
-    <row r="44" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="44" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B44" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="V44" s="28">
+      <c r="U44" s="1">
+        <v>176.4</v>
+      </c>
+      <c r="V44" s="18">
+        <v>217</v>
+      </c>
+      <c r="W44" s="18">
         <v>258.2</v>
       </c>
-      <c r="W44" s="28">
+      <c r="X44" s="18">
         <v>299.60000000000002</v>
       </c>
     </row>
-    <row r="45" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="45" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B45" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="V45" s="28">
+      <c r="U45" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="V45" s="18">
         <v>0</v>
       </c>
-      <c r="W45" s="28">
+      <c r="W45" s="18">
+        <v>0</v>
+      </c>
+      <c r="X45" s="18">
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="46" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B46" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="V46" s="28">
+      <c r="U46" s="1">
+        <v>15.1</v>
+      </c>
+      <c r="V46" s="18">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="W46" s="18">
         <v>24.5</v>
       </c>
-      <c r="W46" s="28">
+      <c r="X46" s="18">
         <v>20.5</v>
       </c>
     </row>
-    <row r="47" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="47" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B47" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="V47" s="28">
+      <c r="U47" s="18">
+        <f>SUM(U41:U46)</f>
+        <v>214.70000000000002</v>
+      </c>
+      <c r="V47" s="18">
         <f>SUM(V41:V46)</f>
+        <v>311.2</v>
+      </c>
+      <c r="W47" s="18">
+        <f>SUM(W41:W46)</f>
         <v>352.2</v>
       </c>
-      <c r="W47" s="28">
-        <f>SUM(W41:W46)</f>
+      <c r="X47" s="18">
+        <f>SUM(X41:X46)</f>
         <v>399.3</v>
       </c>
     </row>
-    <row r="48" spans="2:23" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="2:24" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B48" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D48" s="49"/>
-      <c r="F48" s="49"/>
-      <c r="H48" s="49"/>
-      <c r="J48" s="49"/>
-      <c r="L48" s="49"/>
-      <c r="N48" s="49"/>
-      <c r="P48" s="49"/>
-      <c r="V48" s="37">
+      <c r="D48" s="36"/>
+      <c r="F48" s="36"/>
+      <c r="H48" s="36"/>
+      <c r="J48" s="36"/>
+      <c r="L48" s="36"/>
+      <c r="N48" s="36"/>
+      <c r="P48" s="36"/>
+      <c r="U48" s="2">
+        <v>73.099999999999994</v>
+      </c>
+      <c r="V48" s="27">
+        <v>179.1</v>
+      </c>
+      <c r="W48" s="27">
         <v>0</v>
       </c>
-      <c r="W48" s="37">
+      <c r="X48" s="27">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="49" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B49" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="V49" s="28">
+      <c r="U49" s="1">
+        <v>0</v>
+      </c>
+      <c r="V49" s="18">
+        <v>332.8</v>
+      </c>
+      <c r="W49" s="18">
         <v>280.89999999999998</v>
       </c>
-      <c r="W49" s="28">
+      <c r="X49" s="18">
         <v>316.5</v>
       </c>
     </row>
-    <row r="50" spans="2:23" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="2:24" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B50" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D50" s="49"/>
-      <c r="F50" s="49"/>
-      <c r="H50" s="49"/>
-      <c r="J50" s="49"/>
-      <c r="L50" s="49"/>
-      <c r="N50" s="49"/>
-      <c r="P50" s="49"/>
-      <c r="V50" s="37">
+      <c r="D50" s="36"/>
+      <c r="F50" s="36"/>
+      <c r="H50" s="36"/>
+      <c r="J50" s="36"/>
+      <c r="L50" s="36"/>
+      <c r="N50" s="36"/>
+      <c r="P50" s="36"/>
+      <c r="U50" s="2">
+        <v>0</v>
+      </c>
+      <c r="V50" s="27">
+        <v>0</v>
+      </c>
+      <c r="W50" s="27">
         <v>0.4</v>
       </c>
-      <c r="W50" s="37">
+      <c r="X50" s="27">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="51" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B51" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="V51" s="28">
+      <c r="U51" s="1">
+        <v>28.1</v>
+      </c>
+      <c r="V51" s="18">
+        <v>1.9</v>
+      </c>
+      <c r="W51" s="18">
         <v>3.3</v>
       </c>
-      <c r="W51" s="28">
+      <c r="X51" s="18">
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="52" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="52" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B52" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="V52" s="28">
+      <c r="U52" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="V52" s="18">
         <v>0</v>
       </c>
-      <c r="W52" s="28">
+      <c r="W52" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="2:23" x14ac:dyDescent="0.15">
+      <c r="X52" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B53" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="V53" s="28">
+      <c r="U53" s="1">
+        <v>5.2</v>
+      </c>
+      <c r="V53" s="18">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="W53" s="18">
         <v>15</v>
       </c>
-      <c r="W53" s="28">
+      <c r="X53" s="18">
         <v>6.4</v>
       </c>
     </row>
-    <row r="54" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="54" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B54" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="V54" s="28">
+      <c r="U54" s="18">
+        <f>SUM(U47:U53)</f>
+        <v>321.20000000000005</v>
+      </c>
+      <c r="V54" s="18">
         <f>SUM(V47:V53)</f>
+        <v>829.09999999999991</v>
+      </c>
+      <c r="W54" s="18">
+        <f>SUM(W47:W53)</f>
         <v>651.79999999999984</v>
       </c>
-      <c r="W54" s="28">
-        <f>SUM(W47:W53)</f>
+      <c r="X54" s="18">
+        <f>SUM(X47:X53)</f>
         <v>727.09999999999991</v>
       </c>
     </row>
-    <row r="56" spans="2:23" s="28" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B56" s="28" t="s">
+    <row r="56" spans="2:24" s="18" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B56" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="D56" s="51"/>
-      <c r="F56" s="51"/>
-      <c r="H56" s="51"/>
-      <c r="J56" s="51"/>
-      <c r="L56" s="51"/>
-      <c r="N56" s="51"/>
-      <c r="P56" s="51"/>
-      <c r="V56" s="28">
+      <c r="D56" s="38"/>
+      <c r="F56" s="38"/>
+      <c r="H56" s="38"/>
+      <c r="J56" s="38"/>
+      <c r="L56" s="38"/>
+      <c r="N56" s="38"/>
+      <c r="P56" s="38"/>
+      <c r="U56" s="18">
+        <v>409.3</v>
+      </c>
+      <c r="V56" s="18">
+        <v>365.8</v>
+      </c>
+      <c r="W56" s="18">
         <v>417.8</v>
       </c>
-      <c r="W56" s="28">
+      <c r="X56" s="18">
         <v>551</v>
       </c>
     </row>
-    <row r="57" spans="2:23" s="28" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B57" s="28" t="s">
+    <row r="57" spans="2:24" s="18" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B57" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="D57" s="51"/>
-      <c r="F57" s="51"/>
-      <c r="H57" s="51"/>
-      <c r="J57" s="51"/>
-      <c r="L57" s="51"/>
-      <c r="N57" s="51"/>
-      <c r="P57" s="51"/>
-      <c r="V57" s="28">
+      <c r="D57" s="38"/>
+      <c r="F57" s="38"/>
+      <c r="H57" s="38"/>
+      <c r="J57" s="38"/>
+      <c r="L57" s="38"/>
+      <c r="N57" s="38"/>
+      <c r="P57" s="38"/>
+      <c r="U57" s="18">
+        <f>U56+U54</f>
+        <v>730.5</v>
+      </c>
+      <c r="V57" s="18">
         <f>V56+V54</f>
+        <v>1194.8999999999999</v>
+      </c>
+      <c r="W57" s="18">
+        <f>W56+W54</f>
         <v>1069.5999999999999</v>
       </c>
-      <c r="W57" s="28">
-        <f>W56+W54</f>
+      <c r="X57" s="18">
+        <f>X56+X54</f>
         <v>1278.0999999999999</v>
       </c>
     </row>
-    <row r="59" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="59" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B59" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="V59" s="28">
-        <f t="shared" ref="V59:W59" si="6">V39-V54</f>
+      <c r="U59" s="18">
+        <f t="shared" ref="U59:V59" si="10">U39-U54</f>
+        <v>409.29999999999995</v>
+      </c>
+      <c r="V59" s="18">
+        <f t="shared" ref="V59:W59" si="11">V39-V54</f>
+        <v>365.80000000000018</v>
+      </c>
+      <c r="W59" s="18">
+        <f t="shared" si="11"/>
         <v>417.8000000000003</v>
       </c>
-      <c r="W59" s="28">
-        <f>W39-W54</f>
+      <c r="X59" s="18">
+        <f>X39-X54</f>
         <v>551</v>
       </c>
     </row>
-    <row r="60" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="60" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B60" s="1" t="s">
         <v>101</v>
       </c>
+      <c r="U60" s="1">
+        <f t="shared" ref="U60:V60" si="12">U59/U14</f>
+        <v>2.0557508789552985</v>
+      </c>
       <c r="V60" s="1">
-        <f t="shared" ref="V60" si="7">V59/V14</f>
+        <f t="shared" ref="V60:W60" si="13">V59/V14</f>
+        <v>1.8372677046710206</v>
+      </c>
+      <c r="W60" s="1">
+        <f t="shared" si="13"/>
         <v>2.0984429934706195</v>
       </c>
-      <c r="W60" s="1">
-        <f>W59/W14</f>
+      <c r="X60" s="1">
+        <f>X59/X14</f>
         <v>2.6786582401555665</v>
       </c>
     </row>
-    <row r="62" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="62" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B62" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="V62" s="28">
-        <f t="shared" ref="V62:W62" si="8">V30+V36+V38</f>
+      <c r="U62" s="18">
+        <f t="shared" ref="U62:V62" si="14">U30+U36+U38</f>
+        <v>13</v>
+      </c>
+      <c r="V62" s="18">
+        <f t="shared" ref="V62:W62" si="15">V30+V36+V38</f>
+        <v>124.2</v>
+      </c>
+      <c r="W62" s="18">
+        <f t="shared" si="15"/>
         <v>67.8</v>
       </c>
-      <c r="W62" s="28">
-        <f>W30+W36+W38</f>
+      <c r="X62" s="18">
+        <f>X30+X36+X38</f>
         <v>50.5</v>
       </c>
     </row>
-    <row r="63" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="63" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B63" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="V63" s="28">
-        <f t="shared" ref="V63:W63" si="9">V41+V43+V48+V50</f>
+      <c r="U63" s="18">
+        <f t="shared" ref="U63:V63" si="16">U41+U43+U48+U50</f>
+        <v>93</v>
+      </c>
+      <c r="V63" s="18">
+        <f t="shared" ref="V63:W63" si="17">V41+V43+V48+V50</f>
+        <v>180.4</v>
+      </c>
+      <c r="W63" s="18">
+        <f t="shared" si="17"/>
         <v>6.5000000000000009</v>
       </c>
-      <c r="W63" s="28">
-        <f>W41+W43+W48+W50</f>
+      <c r="X63" s="18">
+        <f>X41+X43+X48+X50</f>
         <v>0.7</v>
       </c>
     </row>
-    <row r="64" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="64" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B64" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="V64" s="28">
-        <f t="shared" ref="V64" si="10">V62-V63</f>
+      <c r="U64" s="18">
+        <f t="shared" ref="U64:V64" si="18">U62-U63</f>
+        <v>-80</v>
+      </c>
+      <c r="V64" s="18">
+        <f t="shared" ref="V64:W64" si="19">V62-V63</f>
+        <v>-56.2</v>
+      </c>
+      <c r="W64" s="18">
+        <f t="shared" si="19"/>
         <v>61.3</v>
       </c>
-      <c r="W64" s="28">
-        <f>W62-W63</f>
+      <c r="X64" s="18">
+        <f>X62-X63</f>
         <v>49.8</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B66" s="1" t="s">
+    <row r="66" spans="2:24" s="30" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B66" s="30" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B68" s="1" t="s">
+      <c r="D66" s="55"/>
+      <c r="F66" s="55"/>
+      <c r="H66" s="55"/>
+      <c r="J66" s="55"/>
+      <c r="L66" s="55"/>
+      <c r="N66" s="55"/>
+      <c r="P66" s="55"/>
+      <c r="V66" s="30">
+        <f>V33/U33-1</f>
+        <v>-4.029936672423684E-3</v>
+      </c>
+      <c r="W66" s="30">
+        <f>W33/V33-1</f>
+        <v>-0.16820809248554913</v>
+      </c>
+      <c r="X66" s="30">
+        <f>X33/W33-1</f>
+        <v>0.54343293954134797</v>
+      </c>
+    </row>
+    <row r="68" spans="2:24" s="53" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B68" s="53" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="D68" s="54"/>
+      <c r="F68" s="54"/>
+      <c r="H68" s="54"/>
+      <c r="J68" s="54"/>
+      <c r="L68" s="54"/>
+      <c r="N68" s="54"/>
+      <c r="P68" s="54"/>
+      <c r="U68" s="53">
+        <v>1.7</v>
+      </c>
+      <c r="V68" s="53">
+        <v>0.60350000000000004</v>
+      </c>
+      <c r="W68" s="53">
+        <v>3.5316000000000001</v>
+      </c>
+      <c r="X68" s="53">
+        <v>2.4632000000000001</v>
+      </c>
+    </row>
+    <row r="69" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B69" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="U69" s="18">
+        <f t="shared" ref="U69:V69" si="20">U68*U14</f>
+        <v>338.46999999999997</v>
+      </c>
+      <c r="V69" s="18">
+        <f t="shared" si="20"/>
+        <v>120.15685000000001</v>
+      </c>
+      <c r="W69" s="18">
+        <f>W68*W14</f>
+        <v>703.14156000000003</v>
+      </c>
+      <c r="X69" s="18">
+        <f>X68*X14</f>
+        <v>506.68023999999997</v>
+      </c>
+    </row>
+    <row r="70" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B70" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B74" s="41" t="s">
+      <c r="U70" s="18">
+        <f>U69-U64</f>
+        <v>418.46999999999997</v>
+      </c>
+      <c r="V70" s="18">
+        <f>V69-V64</f>
+        <v>176.35685000000001</v>
+      </c>
+      <c r="W70" s="18">
+        <f>W69-W64</f>
+        <v>641.84156000000007</v>
+      </c>
+      <c r="X70" s="18">
+        <f>X69-X64</f>
+        <v>456.88023999999996</v>
+      </c>
+    </row>
+    <row r="72" spans="2:24" x14ac:dyDescent="0.15">
+      <c r="B72" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="U72" s="56">
+        <f t="shared" ref="U72:X72" si="21">U68/U60</f>
+        <v>0.82694844857073058</v>
+      </c>
+      <c r="V72" s="56">
+        <f t="shared" si="21"/>
+        <v>0.32847689994532514</v>
+      </c>
+      <c r="W72" s="56">
+        <f t="shared" si="21"/>
+        <v>1.682962087123024</v>
+      </c>
+      <c r="X72" s="56">
+        <f>X68/X60</f>
+        <v>0.91956486388384751</v>
+      </c>
+    </row>
+    <row r="73" spans="2:24" s="56" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B73" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="D73" s="57"/>
+      <c r="F73" s="57"/>
+      <c r="H73" s="57"/>
+      <c r="J73" s="57"/>
+      <c r="L73" s="57"/>
+      <c r="N73" s="57"/>
+      <c r="P73" s="57"/>
+      <c r="U73" s="56">
+        <f t="shared" ref="U73:X73" si="22">U69/U4</f>
+        <v>0.29726857544352714</v>
+      </c>
+      <c r="V73" s="56">
+        <f t="shared" si="22"/>
+        <v>0.10402289845035063</v>
+      </c>
+      <c r="W73" s="56">
+        <f t="shared" si="22"/>
+        <v>0.54410087440996679</v>
+      </c>
+      <c r="X73" s="56">
+        <f>X69/X4</f>
+        <v>0.36994760514018693</v>
+      </c>
+    </row>
+    <row r="74" spans="2:24" s="56" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B74" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="D74" s="57"/>
+      <c r="F74" s="57"/>
+      <c r="H74" s="57"/>
+      <c r="J74" s="57"/>
+      <c r="L74" s="57"/>
+      <c r="N74" s="57"/>
+      <c r="P74" s="57"/>
+      <c r="U74" s="56">
+        <f t="shared" ref="U74:X74" si="23">U70/U4</f>
+        <v>0.36753030036887407</v>
+      </c>
+      <c r="V74" s="56">
+        <f t="shared" si="23"/>
+        <v>0.15267669465847114</v>
+      </c>
+      <c r="W74" s="56">
+        <f t="shared" si="23"/>
+        <v>0.49666606825040632</v>
+      </c>
+      <c r="X74" s="56">
+        <f>X70/X4</f>
+        <v>0.33358662383177567</v>
+      </c>
+    </row>
+    <row r="75" spans="2:24" s="56" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B75" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="D75" s="57"/>
+      <c r="F75" s="57"/>
+      <c r="H75" s="57"/>
+      <c r="J75" s="57"/>
+      <c r="L75" s="57"/>
+      <c r="N75" s="57"/>
+      <c r="P75" s="57"/>
+      <c r="U75" s="56">
+        <f t="shared" ref="U75:X75" si="24">U68/U13</f>
+        <v>8.0780429594272327</v>
+      </c>
+      <c r="V75" s="56">
+        <f t="shared" si="24"/>
+        <v>6.8661057142857596</v>
+      </c>
+      <c r="W75" s="56">
+        <f t="shared" si="24"/>
+        <v>13.216946616541351</v>
+      </c>
+      <c r="X75" s="56">
+        <f>X68/X13</f>
+        <v>6.520981209781211</v>
+      </c>
+    </row>
+    <row r="76" spans="2:24" s="56" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B76" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="D76" s="57"/>
+      <c r="F76" s="57"/>
+      <c r="H76" s="57"/>
+      <c r="J76" s="57"/>
+      <c r="L76" s="57"/>
+      <c r="N76" s="57"/>
+      <c r="P76" s="57"/>
+      <c r="U76" s="56">
+        <f t="shared" ref="U76:X76" si="25">U70/U12</f>
+        <v>9.9873508353222267</v>
+      </c>
+      <c r="V76" s="56">
+        <f t="shared" si="25"/>
+        <v>10.077534285714352</v>
+      </c>
+      <c r="W76" s="56">
+        <f t="shared" si="25"/>
+        <v>12.064690977443609</v>
+      </c>
+      <c r="X76" s="56">
+        <f>X70/X12</f>
+        <v>5.8800545688545691</v>
+      </c>
+    </row>
+    <row r="79" spans="2:24" x14ac:dyDescent="0.15">
+      <c r="B79" s="31" t="s">
         <v>107</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="W1" r:id="rId1" xr:uid="{596F9973-92FB-3340-BC7A-375E4C25351C}"/>
+    <hyperlink ref="X1" r:id="rId1" xr:uid="{596F9973-92FB-3340-BC7A-375E4C25351C}"/>
+    <hyperlink ref="V1" r:id="rId2" xr:uid="{92846B6F-2839-284E-AA85-90B408C1E203}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
+  <ignoredErrors>
+    <ignoredError sqref="V9" formula="1"/>
+  </ignoredErrors>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
£HFD latest interim results
</commit_message>
<xml_diff>
--- a/£HFD.xlsx
+++ b/£HFD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20404"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0775040A-AD96-4D70-8B9A-2B5BB1F71BAB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4531BF89-C0E8-4459-84BB-A4FD8B5851BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3483339E-0186-4DD8-B843-20C8BDA2099F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{3483339E-0186-4DD8-B843-20C8BDA2099F}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -631,7 +631,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -751,25 +751,13 @@
     <xf numFmtId="16" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -780,7 +768,19 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -789,15 +789,19 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="17" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="16" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -936,14 +940,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>22225</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>22225</xdr:colOff>
       <xdr:row>106</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
@@ -960,8 +964,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9880600" y="0"/>
-          <a:ext cx="0" cy="16548100"/>
+          <a:off x="9899650" y="0"/>
+          <a:ext cx="0" cy="17202150"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1286,8 +1290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ACB5AEF-8447-4D06-8D6B-C9C6F674AB9E}">
   <dimension ref="B2:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1314,22 +1318,22 @@
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B5" s="77" t="s">
+      <c r="B5" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="78"/>
-      <c r="D5" s="79"/>
-      <c r="G5" s="77" t="s">
+      <c r="C5" s="83"/>
+      <c r="D5" s="84"/>
+      <c r="G5" s="82" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="78"/>
-      <c r="I5" s="78"/>
-      <c r="J5" s="78"/>
-      <c r="K5" s="78"/>
-      <c r="L5" s="78"/>
-      <c r="M5" s="78"/>
-      <c r="N5" s="78"/>
-      <c r="O5" s="79"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="83"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="83"/>
+      <c r="L5" s="83"/>
+      <c r="M5" s="83"/>
+      <c r="N5" s="83"/>
+      <c r="O5" s="84"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
@@ -1339,7 +1343,7 @@
         <v>1.829</v>
       </c>
       <c r="D6" s="15"/>
-      <c r="G6" s="89"/>
+      <c r="G6" s="75"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
@@ -1360,7 +1364,7 @@
         <f>C29</f>
         <v>FY22</v>
       </c>
-      <c r="G7" s="91">
+      <c r="G7" s="77">
         <v>45200</v>
       </c>
       <c r="H7" s="6" t="s">
@@ -1383,7 +1387,7 @@
         <v>376.22529999999995</v>
       </c>
       <c r="D8" s="15"/>
-      <c r="G8" s="89"/>
+      <c r="G8" s="75"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
@@ -1405,7 +1409,7 @@
         <f>$C$29</f>
         <v>FY22</v>
       </c>
-      <c r="G9" s="89"/>
+      <c r="G9" s="75"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
@@ -1427,7 +1431,7 @@
         <f>$C$29</f>
         <v>FY22</v>
       </c>
-      <c r="G10" s="89"/>
+      <c r="G10" s="75"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
@@ -1449,7 +1453,7 @@
         <f>$C$29</f>
         <v>FY22</v>
       </c>
-      <c r="G11" s="89"/>
+      <c r="G11" s="75"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
@@ -1468,7 +1472,7 @@
         <v>326.42529999999994</v>
       </c>
       <c r="D12" s="16"/>
-      <c r="G12" s="89"/>
+      <c r="G12" s="75"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
@@ -1479,7 +1483,7 @@
       <c r="O12" s="7"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="G13" s="89"/>
+      <c r="G13" s="75"/>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
@@ -1490,7 +1494,7 @@
       <c r="O13" s="7"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="G14" s="89"/>
+      <c r="G14" s="75"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
@@ -1501,12 +1505,12 @@
       <c r="O14" s="7"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B15" s="77" t="s">
+      <c r="B15" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="78"/>
-      <c r="D15" s="79"/>
-      <c r="G15" s="89"/>
+      <c r="C15" s="83"/>
+      <c r="D15" s="84"/>
+      <c r="G15" s="75"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
@@ -1520,11 +1524,11 @@
       <c r="B16" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="80" t="s">
+      <c r="C16" s="91" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="81"/>
-      <c r="G16" s="89"/>
+      <c r="D16" s="86"/>
+      <c r="G16" s="75"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
@@ -1538,11 +1542,11 @@
       <c r="B17" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="80" t="s">
+      <c r="C17" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="81"/>
-      <c r="G17" s="89"/>
+      <c r="D17" s="86"/>
+      <c r="G17" s="75"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
@@ -1556,11 +1560,11 @@
       <c r="B18" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="80" t="s">
+      <c r="C18" s="91" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="81"/>
-      <c r="G18" s="89"/>
+      <c r="D18" s="86"/>
+      <c r="G18" s="75"/>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
@@ -1574,11 +1578,11 @@
       <c r="B19" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="75" t="s">
+      <c r="C19" s="89" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="76"/>
-      <c r="G19" s="90"/>
+      <c r="D19" s="90"/>
+      <c r="G19" s="76"/>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
@@ -1589,61 +1593,61 @@
       <c r="O19" s="10"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B22" s="77" t="s">
+      <c r="B22" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="78"/>
-      <c r="D22" s="79"/>
+      <c r="C22" s="83"/>
+      <c r="D22" s="84"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B23" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="86" t="s">
+      <c r="C23" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="81"/>
+      <c r="D23" s="86"/>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B24" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="86">
+      <c r="C24" s="85">
         <v>1892</v>
       </c>
-      <c r="D24" s="81"/>
+      <c r="D24" s="86"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B25" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="86">
+      <c r="C25" s="85">
         <v>2004</v>
       </c>
-      <c r="D25" s="81"/>
+      <c r="D25" s="86"/>
       <c r="E25" s="1" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B26" s="11"/>
-      <c r="C26" s="86"/>
-      <c r="D26" s="81"/>
+      <c r="C26" s="85"/>
+      <c r="D26" s="86"/>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B27" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="86">
+      <c r="C27" s="85">
         <f>'Financial Model'!Z34</f>
         <v>222.1</v>
       </c>
-      <c r="D27" s="81"/>
+      <c r="D27" s="86"/>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B28" s="11"/>
-      <c r="C28" s="86"/>
-      <c r="D28" s="81"/>
+      <c r="C28" s="85"/>
+      <c r="D28" s="86"/>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B29" s="11" t="s">
@@ -1667,76 +1671,82 @@
       <c r="D30" s="88"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B33" s="77" t="s">
+      <c r="B33" s="82" t="s">
         <v>20</v>
       </c>
-      <c r="C33" s="78"/>
-      <c r="D33" s="79"/>
+      <c r="C33" s="83"/>
+      <c r="D33" s="84"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B34" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C34" s="82">
+      <c r="C34" s="78">
         <f>C6/'Financial Model'!Z61</f>
         <v>0.68280453720508161</v>
       </c>
-      <c r="D34" s="83"/>
+      <c r="D34" s="79"/>
       <c r="E34" s="29"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B35" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C35" s="82">
+      <c r="C35" s="78">
         <f>C8/'Financial Model'!Z4</f>
         <v>0.27469721086448595</v>
       </c>
-      <c r="D35" s="83"/>
+      <c r="D35" s="79"/>
       <c r="E35" s="29"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B36" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="82">
+      <c r="C36" s="78">
         <f>C12/'Financial Model'!Z4</f>
         <v>0.23833622955607472</v>
       </c>
-      <c r="D36" s="83"/>
+      <c r="D36" s="79"/>
       <c r="E36" s="29"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B37" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C37" s="82">
+      <c r="C37" s="78">
         <f>C6/'Financial Model'!Z13</f>
         <v>4.8420244530244538</v>
       </c>
-      <c r="D37" s="83"/>
+      <c r="D37" s="79"/>
       <c r="E37" s="29"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B38" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C38" s="82">
+      <c r="C38" s="78">
         <f>C12/'Financial Model'!Z12</f>
         <v>4.201097812097812</v>
       </c>
-      <c r="D38" s="83"/>
+      <c r="D38" s="79"/>
       <c r="E38" s="29"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B39" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="C39" s="84"/>
-      <c r="D39" s="85"/>
+      <c r="C39" s="80"/>
+      <c r="D39" s="81"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="C37:D37"/>
     <mergeCell ref="C38:D38"/>
@@ -1753,12 +1763,6 @@
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C30:D30" r:id="rId1" display="Link" xr:uid="{07676FE1-E26A-AE4D-A21B-792EB2B848FD}"/>
@@ -1773,11 +1777,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFF52FD5-5387-455B-8CDC-129D27EFA8D5}">
   <dimension ref="A1:CS80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AA69" sqref="AA69"/>
+      <selection pane="bottomRight" activeCell="M73" sqref="M73:O73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1843,7 +1847,7 @@
       <c r="N1" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="O1" s="20" t="s">
+      <c r="O1" s="25" t="s">
         <v>46</v>
       </c>
       <c r="P1" s="32" t="s">
@@ -1916,7 +1920,13 @@
         <v>44470</v>
       </c>
       <c r="L2" s="33"/>
+      <c r="M2" s="24">
+        <v>44834</v>
+      </c>
       <c r="N2" s="33"/>
+      <c r="O2" s="24">
+        <v>45198</v>
+      </c>
       <c r="P2" s="33"/>
       <c r="S2" s="24">
         <v>42097</v>
@@ -1968,6 +1978,9 @@
         <v>44868</v>
       </c>
       <c r="N3" s="33"/>
+      <c r="O3" s="92">
+        <v>45259</v>
+      </c>
       <c r="P3" s="33"/>
       <c r="T3" s="23">
         <v>42522</v>
@@ -1995,7 +2008,13 @@
       <c r="H4" s="34"/>
       <c r="J4" s="34"/>
       <c r="L4" s="34"/>
+      <c r="M4" s="2">
+        <v>767.1</v>
+      </c>
       <c r="N4" s="34"/>
+      <c r="O4" s="2">
+        <v>873.5</v>
+      </c>
       <c r="P4" s="34"/>
       <c r="S4" s="26">
         <v>1025.4000000000001</v>
@@ -2061,6 +2080,12 @@
     <row r="5" spans="2:97" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>65</v>
+      </c>
+      <c r="M5" s="1">
+        <v>384.6</v>
+      </c>
+      <c r="O5" s="1">
+        <v>456.2</v>
       </c>
       <c r="S5" s="17">
         <v>479.1</v>
@@ -2132,7 +2157,15 @@
       <c r="H6" s="34"/>
       <c r="J6" s="34"/>
       <c r="L6" s="34"/>
+      <c r="M6" s="2">
+        <f>M4-M5</f>
+        <v>382.5</v>
+      </c>
       <c r="N6" s="34"/>
+      <c r="O6" s="2">
+        <f>O4-O5</f>
+        <v>417.3</v>
+      </c>
       <c r="P6" s="34"/>
       <c r="S6" s="26">
         <f t="shared" ref="S6:V6" si="2">S4-S5</f>
@@ -2206,6 +2239,14 @@
     <row r="7" spans="2:97" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>67</v>
+      </c>
+      <c r="M7" s="1">
+        <f>358.7-0.3</f>
+        <v>358.4</v>
+      </c>
+      <c r="O7" s="1">
+        <f>389.7+2</f>
+        <v>391.7</v>
       </c>
       <c r="S7" s="17">
         <v>459</v>
@@ -2277,7 +2318,15 @@
       <c r="H8" s="34"/>
       <c r="J8" s="34"/>
       <c r="L8" s="34"/>
+      <c r="M8" s="2">
+        <f>M6-M7</f>
+        <v>24.100000000000023</v>
+      </c>
       <c r="N8" s="34"/>
+      <c r="O8" s="2">
+        <f>O6-O7</f>
+        <v>25.600000000000023</v>
+      </c>
       <c r="P8" s="34"/>
       <c r="S8" s="26">
         <f t="shared" ref="S8:V8" si="6">S6-S7</f>
@@ -2352,6 +2401,12 @@
       <c r="B9" s="1" t="s">
         <v>69</v>
       </c>
+      <c r="M9" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="O9" s="1">
+        <v>6.3</v>
+      </c>
       <c r="S9" s="17">
         <v>3.5</v>
       </c>
@@ -2418,6 +2473,14 @@
       <c r="B10" s="1" t="s">
         <v>70</v>
       </c>
+      <c r="M10" s="1">
+        <f>M8-M9</f>
+        <v>18.700000000000024</v>
+      </c>
+      <c r="O10" s="1">
+        <f>O8-O9</f>
+        <v>19.300000000000022</v>
+      </c>
       <c r="S10" s="17">
         <f t="shared" ref="S10:V10" si="9">S8-S9</f>
         <v>83.800000000000068</v>
@@ -2490,6 +2553,13 @@
     <row r="11" spans="2:97" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>71</v>
+      </c>
+      <c r="M11" s="1">
+        <f>3.8+0.2</f>
+        <v>4</v>
+      </c>
+      <c r="O11" s="1">
+        <v>4.7</v>
       </c>
       <c r="S11" s="17">
         <v>18</v>
@@ -2561,7 +2631,15 @@
       <c r="H12" s="34"/>
       <c r="J12" s="34"/>
       <c r="L12" s="34"/>
+      <c r="M12" s="2">
+        <f>M10-M11</f>
+        <v>14.700000000000024</v>
+      </c>
       <c r="N12" s="34"/>
+      <c r="O12" s="2">
+        <f>O10-O11</f>
+        <v>14.600000000000023</v>
+      </c>
       <c r="P12" s="34"/>
       <c r="S12" s="26">
         <f t="shared" ref="S12:V12" si="12">S10-S11</f>
@@ -2880,10 +2958,25 @@
         <v>32.188263512376381</v>
       </c>
     </row>
-    <row r="13" spans="2:97" x14ac:dyDescent="0.2">
-      <c r="B13" s="1" t="s">
+    <row r="13" spans="2:97" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="27" t="s">
         <v>62</v>
       </c>
+      <c r="D13" s="93"/>
+      <c r="F13" s="93"/>
+      <c r="H13" s="93"/>
+      <c r="J13" s="93"/>
+      <c r="L13" s="93"/>
+      <c r="M13" s="27">
+        <f>M12/M14</f>
+        <v>6.5566458519179416E-2</v>
+      </c>
+      <c r="N13" s="93"/>
+      <c r="O13" s="27">
+        <f>O12/O14</f>
+        <v>6.4345526663728614E-2</v>
+      </c>
+      <c r="P13" s="93"/>
       <c r="S13" s="27">
         <f t="shared" ref="S13:U13" si="15">S12/S14</f>
         <v>0.33333333333333365</v>
@@ -2956,6 +3049,12 @@
     <row r="14" spans="2:97" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="M14" s="1">
+        <v>224.2</v>
+      </c>
+      <c r="O14" s="1">
+        <v>226.9</v>
       </c>
       <c r="S14" s="1">
         <v>197.4</v>
@@ -3028,6 +3127,10 @@
       <c r="J16" s="34"/>
       <c r="L16" s="34"/>
       <c r="N16" s="34"/>
+      <c r="O16" s="28">
+        <f>O4/M4-1</f>
+        <v>0.13870421066353789</v>
+      </c>
       <c r="P16" s="34"/>
       <c r="T16" s="28">
         <f t="shared" ref="T16" si="20">T4/S4-1</f>
@@ -3118,6 +3221,15 @@
       <c r="B19" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="M19" s="29">
+        <f>M6/M4</f>
+        <v>0.49863120844739928</v>
+      </c>
+      <c r="N19" s="40"/>
+      <c r="O19" s="29">
+        <f>O6/O4</f>
+        <v>0.47773325701202063</v>
+      </c>
       <c r="S19" s="29">
         <f t="shared" ref="S19:T19" si="23">S6/S4</f>
         <v>0.53276770040959631</v>
@@ -3188,6 +3300,15 @@
       <c r="B20" s="1" t="s">
         <v>75</v>
       </c>
+      <c r="M20" s="29">
+        <f>M8/M4</f>
+        <v>3.1417025159692379E-2</v>
+      </c>
+      <c r="N20" s="40"/>
+      <c r="O20" s="29">
+        <f>O8/O4</f>
+        <v>2.9307384087006321E-2</v>
+      </c>
       <c r="S20" s="29">
         <f t="shared" ref="S20:T20" si="26">S8/S4</f>
         <v>8.5137507314218902E-2</v>
@@ -3267,6 +3388,15 @@
       <c r="B21" s="1" t="s">
         <v>76</v>
       </c>
+      <c r="M21" s="29">
+        <f>M12/M4</f>
+        <v>1.9163081736409886E-2</v>
+      </c>
+      <c r="N21" s="40"/>
+      <c r="O21" s="29">
+        <f>O12/O4</f>
+        <v>1.6714367487120803E-2</v>
+      </c>
       <c r="S21" s="29">
         <f t="shared" ref="S21:T21" si="30">S12/S4</f>
         <v>6.4170079968792731E-2</v>
@@ -3347,6 +3477,15 @@
       <c r="B22" s="1" t="s">
         <v>77</v>
       </c>
+      <c r="M22" s="29">
+        <f>M11/M10</f>
+        <v>0.21390374331550774</v>
+      </c>
+      <c r="N22" s="40"/>
+      <c r="O22" s="29">
+        <f>O11/O10</f>
+        <v>0.24352331606217589</v>
+      </c>
       <c r="S22" s="29">
         <f t="shared" ref="S22:T22" si="34">S11/S10</f>
         <v>0.21479713603818598</v>
@@ -3465,6 +3604,12 @@
       <c r="B27" s="1" t="s">
         <v>80</v>
       </c>
+      <c r="M27" s="17">
+        <v>444.7</v>
+      </c>
+      <c r="O27" s="17">
+        <v>481.6</v>
+      </c>
       <c r="S27" s="1">
         <v>356.8</v>
       </c>
@@ -3494,6 +3639,12 @@
       <c r="B28" s="1" t="s">
         <v>81</v>
       </c>
+      <c r="M28" s="17">
+        <v>97.9</v>
+      </c>
+      <c r="O28" s="17">
+        <v>92.8</v>
+      </c>
       <c r="S28" s="1">
         <v>103.8</v>
       </c>
@@ -3522,6 +3673,12 @@
     <row r="29" spans="2:38" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
         <v>82</v>
+      </c>
+      <c r="M29" s="17">
+        <v>329.8</v>
+      </c>
+      <c r="O29" s="17">
+        <v>294.5</v>
       </c>
       <c r="S29" s="17">
         <v>0</v>
@@ -3557,7 +3714,13 @@
       <c r="H30" s="34"/>
       <c r="J30" s="34"/>
       <c r="L30" s="34"/>
+      <c r="M30" s="26">
+        <v>0.7</v>
+      </c>
       <c r="N30" s="34"/>
+      <c r="O30" s="26">
+        <v>0.3</v>
+      </c>
       <c r="P30" s="34"/>
       <c r="S30" s="26">
         <v>0</v>
@@ -3597,6 +3760,12 @@
       <c r="B31" s="1" t="s">
         <v>84</v>
       </c>
+      <c r="M31" s="17">
+        <v>13.1</v>
+      </c>
+      <c r="O31" s="17">
+        <v>9</v>
+      </c>
       <c r="S31" s="1">
         <v>4.0999999999999996</v>
       </c>
@@ -3626,6 +3795,12 @@
       <c r="B32" s="1" t="s">
         <v>112</v>
       </c>
+      <c r="M32" s="17">
+        <v>0</v>
+      </c>
+      <c r="O32" s="17">
+        <v>0</v>
+      </c>
       <c r="S32" s="17">
         <v>0</v>
       </c>
@@ -3654,6 +3829,14 @@
     <row r="33" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
         <v>85</v>
+      </c>
+      <c r="M33" s="17">
+        <f>SUM(M27:M32)</f>
+        <v>886.20000000000016</v>
+      </c>
+      <c r="O33" s="17">
+        <f>SUM(O27:O32)</f>
+        <v>878.19999999999993</v>
       </c>
       <c r="S33" s="17">
         <f t="shared" ref="S33:Z33" si="38">SUM(S27:S32)</f>
@@ -3697,7 +3880,13 @@
       <c r="H34" s="34"/>
       <c r="J34" s="34"/>
       <c r="L34" s="34"/>
+      <c r="M34" s="26">
+        <v>248</v>
+      </c>
       <c r="N34" s="34"/>
+      <c r="O34" s="26">
+        <v>262.89999999999998</v>
+      </c>
       <c r="P34" s="34"/>
       <c r="S34" s="2">
         <v>149.30000000000001</v>
@@ -3737,6 +3926,12 @@
       <c r="B35" s="1" t="s">
         <v>87</v>
       </c>
+      <c r="M35" s="17">
+        <v>118.2</v>
+      </c>
+      <c r="O35" s="17">
+        <v>162.5</v>
+      </c>
       <c r="S35" s="1">
         <v>55.8</v>
       </c>
@@ -3765,6 +3960,12 @@
     <row r="36" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
         <v>88</v>
+      </c>
+      <c r="M36" s="17">
+        <v>0</v>
+      </c>
+      <c r="O36" s="17">
+        <v>0</v>
       </c>
       <c r="S36" s="17">
         <v>0</v>
@@ -3800,7 +4001,13 @@
       <c r="H37" s="34"/>
       <c r="J37" s="34"/>
       <c r="L37" s="34"/>
+      <c r="M37" s="26">
+        <v>15.7</v>
+      </c>
       <c r="N37" s="34"/>
+      <c r="O37" s="26">
+        <v>1.4</v>
+      </c>
       <c r="P37" s="34"/>
       <c r="S37" s="2">
         <v>3.9</v>
@@ -3840,6 +4047,12 @@
       <c r="B38" s="1" t="s">
         <v>89</v>
       </c>
+      <c r="M38" s="17">
+        <v>1.8</v>
+      </c>
+      <c r="O38" s="17">
+        <v>7.5</v>
+      </c>
       <c r="S38" s="17">
         <v>0</v>
       </c>
@@ -3874,7 +4087,13 @@
       <c r="H39" s="34"/>
       <c r="J39" s="34"/>
       <c r="L39" s="34"/>
+      <c r="M39" s="26">
+        <v>78</v>
+      </c>
       <c r="N39" s="34"/>
+      <c r="O39" s="26">
+        <v>16.2</v>
+      </c>
       <c r="P39" s="34"/>
       <c r="S39" s="2">
         <v>22.4</v>
@@ -3914,6 +4133,14 @@
       <c r="B40" s="1" t="s">
         <v>90</v>
       </c>
+      <c r="M40" s="17">
+        <f>SUM(M33:M39)</f>
+        <v>1347.9000000000003</v>
+      </c>
+      <c r="O40" s="17">
+        <f>SUM(O33:O39)</f>
+        <v>1328.7</v>
+      </c>
       <c r="S40" s="17">
         <f t="shared" ref="S40:Y40" si="39">SUM(S33:S39)</f>
         <v>696.09999999999991</v>
@@ -3948,6 +4175,8 @@
       </c>
     </row>
     <row r="41" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="M41" s="17"/>
+      <c r="O41" s="17"/>
       <c r="Y41" s="17"/>
     </row>
     <row r="42" spans="2:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3959,7 +4188,13 @@
       <c r="H42" s="34"/>
       <c r="J42" s="34"/>
       <c r="L42" s="34"/>
+      <c r="M42" s="26">
+        <v>11.5</v>
+      </c>
       <c r="N42" s="34"/>
+      <c r="O42" s="26">
+        <v>13.8</v>
+      </c>
       <c r="P42" s="34"/>
       <c r="S42" s="2">
         <v>22.9</v>
@@ -3999,6 +4234,12 @@
       <c r="B43" s="1" t="s">
         <v>92</v>
       </c>
+      <c r="M43" s="17">
+        <v>75.2</v>
+      </c>
+      <c r="O43" s="17">
+        <v>71.900000000000006</v>
+      </c>
       <c r="S43" s="17">
         <v>0</v>
       </c>
@@ -4033,7 +4274,13 @@
       <c r="H44" s="34"/>
       <c r="J44" s="34"/>
       <c r="L44" s="34"/>
+      <c r="M44" s="26">
+        <v>0.1</v>
+      </c>
       <c r="N44" s="34"/>
+      <c r="O44" s="26">
+        <v>1.3</v>
+      </c>
       <c r="P44" s="34"/>
       <c r="S44" s="2">
         <v>0.1</v>
@@ -4073,6 +4320,12 @@
       <c r="B45" s="1" t="s">
         <v>93</v>
       </c>
+      <c r="M45" s="17">
+        <v>350.8</v>
+      </c>
+      <c r="O45" s="17">
+        <v>360</v>
+      </c>
       <c r="S45" s="1">
         <v>181.4</v>
       </c>
@@ -4102,6 +4355,12 @@
       <c r="B46" s="1" t="s">
         <v>94</v>
       </c>
+      <c r="M46" s="17">
+        <v>0</v>
+      </c>
+      <c r="O46" s="17">
+        <v>0</v>
+      </c>
       <c r="S46" s="1">
         <v>12.4</v>
       </c>
@@ -4131,6 +4390,12 @@
       <c r="B47" s="1" t="s">
         <v>95</v>
       </c>
+      <c r="M47" s="17">
+        <v>20.3</v>
+      </c>
+      <c r="O47" s="17">
+        <v>13.4</v>
+      </c>
       <c r="S47" s="1">
         <v>10.6</v>
       </c>
@@ -4159,6 +4424,14 @@
     <row r="48" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B48" s="1" t="s">
         <v>96</v>
+      </c>
+      <c r="M48" s="17">
+        <f>SUM(M42:M47)</f>
+        <v>457.90000000000003</v>
+      </c>
+      <c r="O48" s="17">
+        <f>SUM(O42:O47)</f>
+        <v>460.4</v>
       </c>
       <c r="S48" s="17">
         <f t="shared" ref="S48:V48" si="40">SUM(S42:S47)</f>
@@ -4202,7 +4475,13 @@
       <c r="H49" s="34"/>
       <c r="J49" s="34"/>
       <c r="L49" s="34"/>
+      <c r="M49" s="26">
+        <v>34.200000000000003</v>
+      </c>
       <c r="N49" s="34"/>
+      <c r="O49" s="26">
+        <v>49.4</v>
+      </c>
       <c r="P49" s="34"/>
       <c r="S49" s="2">
         <v>61.3</v>
@@ -4242,6 +4521,12 @@
       <c r="B50" s="1" t="s">
         <v>92</v>
       </c>
+      <c r="M50" s="17">
+        <v>293.10000000000002</v>
+      </c>
+      <c r="O50" s="17">
+        <v>253.4</v>
+      </c>
       <c r="S50" s="1">
         <v>31.5</v>
       </c>
@@ -4276,7 +4561,13 @@
       <c r="H51" s="34"/>
       <c r="J51" s="34"/>
       <c r="L51" s="34"/>
+      <c r="M51" s="26">
+        <v>0.1</v>
+      </c>
       <c r="N51" s="34"/>
+      <c r="O51" s="26">
+        <v>0</v>
+      </c>
       <c r="P51" s="34"/>
       <c r="S51" s="26">
         <v>0</v>
@@ -4316,6 +4607,12 @@
       <c r="B52" s="1" t="s">
         <v>93</v>
       </c>
+      <c r="M52" s="26">
+        <v>3.7</v>
+      </c>
+      <c r="O52" s="17">
+        <v>3.9</v>
+      </c>
       <c r="S52" s="17">
         <v>0</v>
       </c>
@@ -4345,6 +4642,12 @@
       <c r="B53" s="1" t="s">
         <v>84</v>
       </c>
+      <c r="M53" s="17">
+        <v>0</v>
+      </c>
+      <c r="O53" s="17">
+        <v>0</v>
+      </c>
       <c r="S53" s="17">
         <v>0</v>
       </c>
@@ -4374,6 +4677,12 @@
       <c r="B54" s="1" t="s">
         <v>95</v>
       </c>
+      <c r="M54" s="17">
+        <v>4.3</v>
+      </c>
+      <c r="O54" s="17">
+        <v>11</v>
+      </c>
       <c r="S54" s="1">
         <v>8.1999999999999993</v>
       </c>
@@ -4403,6 +4712,14 @@
       <c r="B55" s="1" t="s">
         <v>97</v>
       </c>
+      <c r="M55" s="17">
+        <f>SUM(M48:M54)</f>
+        <v>793.30000000000007</v>
+      </c>
+      <c r="O55" s="17">
+        <f>SUM(O48:O54)</f>
+        <v>778.09999999999991</v>
+      </c>
       <c r="S55" s="17">
         <f t="shared" ref="S55:V55" si="41">SUM(S48:S54)</f>
         <v>328.4</v>
@@ -4435,6 +4752,9 @@
         <f>SUM(Z48:Z54)</f>
         <v>727.09999999999991</v>
       </c>
+    </row>
+    <row r="56" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="O56" s="17"/>
     </row>
     <row r="57" spans="2:35" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B57" s="17" t="s">
@@ -4445,7 +4765,13 @@
       <c r="H57" s="36"/>
       <c r="J57" s="36"/>
       <c r="L57" s="36"/>
+      <c r="M57" s="17">
+        <v>554.6</v>
+      </c>
       <c r="N57" s="36"/>
+      <c r="O57" s="17">
+        <v>550.6</v>
+      </c>
       <c r="P57" s="36"/>
       <c r="S57" s="17">
         <v>367.7</v>
@@ -4490,7 +4816,15 @@
       <c r="H58" s="36"/>
       <c r="J58" s="36"/>
       <c r="L58" s="36"/>
+      <c r="M58" s="17">
+        <f>+M57+M55</f>
+        <v>1347.9</v>
+      </c>
       <c r="N58" s="36"/>
+      <c r="O58" s="17">
+        <f>+O57+O55</f>
+        <v>1328.6999999999998</v>
+      </c>
       <c r="P58" s="36"/>
       <c r="S58" s="17">
         <f t="shared" ref="S58:V58" si="42">S57+S55</f>
@@ -4538,6 +4872,14 @@
       <c r="B60" s="1" t="s">
         <v>100</v>
       </c>
+      <c r="M60" s="17">
+        <f>M40-M55</f>
+        <v>554.60000000000025</v>
+      </c>
+      <c r="O60" s="17">
+        <f>O40-O55</f>
+        <v>550.60000000000014</v>
+      </c>
       <c r="S60" s="17">
         <f t="shared" ref="S60:T60" si="43">S40-S55</f>
         <v>367.69999999999993</v>
@@ -4575,6 +4917,14 @@
       <c r="B61" s="1" t="s">
         <v>101</v>
       </c>
+      <c r="M61" s="1">
+        <f>M60/M14</f>
+        <v>2.4736842105263168</v>
+      </c>
+      <c r="O61" s="1">
+        <f>O60/O14</f>
+        <v>2.4266196562362281</v>
+      </c>
       <c r="S61" s="1">
         <f t="shared" ref="S61:T61" si="46">S60/S14</f>
         <v>1.8627152988855114</v>
@@ -4612,32 +4962,40 @@
       <c r="B63" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="M63" s="17">
+        <f t="shared" ref="M63:O63" si="49">M30+M37+M39</f>
+        <v>94.4</v>
+      </c>
+      <c r="O63" s="17">
+        <f t="shared" si="49"/>
+        <v>17.899999999999999</v>
+      </c>
       <c r="S63" s="17">
-        <f t="shared" ref="S63:T63" si="49">S30+S37+S39</f>
+        <f t="shared" ref="S63:T63" si="50">S30+S37+S39</f>
         <v>26.299999999999997</v>
       </c>
       <c r="T63" s="17">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>16.100000000000001</v>
       </c>
       <c r="U63" s="17">
-        <f t="shared" ref="U63:W63" si="50">U30+U37+U39</f>
+        <f t="shared" ref="U63:W63" si="51">U30+U37+U39</f>
         <v>21.7</v>
       </c>
       <c r="V63" s="17">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>27.3</v>
       </c>
       <c r="W63" s="17">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>13</v>
       </c>
       <c r="X63" s="17">
-        <f t="shared" ref="X63:Y63" si="51">X30+X37+X39</f>
+        <f t="shared" ref="X63:Y63" si="52">X30+X37+X39</f>
         <v>124.2</v>
       </c>
       <c r="Y63" s="17">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>67.8</v>
       </c>
       <c r="Z63" s="17">
@@ -4649,32 +5007,40 @@
       <c r="B64" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="M64" s="17">
+        <f t="shared" ref="M64:O64" si="53">M42+M44+M49+M51</f>
+        <v>45.900000000000006</v>
+      </c>
+      <c r="O64" s="17">
+        <f t="shared" si="53"/>
+        <v>64.5</v>
+      </c>
       <c r="S64" s="17">
-        <f t="shared" ref="S64:T64" si="52">S42+S44+S49+S51</f>
+        <f t="shared" ref="S64:T64" si="54">S42+S44+S49+S51</f>
         <v>84.3</v>
       </c>
       <c r="T64" s="17">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>59.8</v>
       </c>
       <c r="U64" s="17">
-        <f t="shared" ref="U64:W64" si="53">U42+U44+U49+U51</f>
+        <f t="shared" ref="U64:W64" si="55">U42+U44+U49+U51</f>
         <v>103.89999999999999</v>
       </c>
       <c r="V64" s="17">
-        <f t="shared" si="53"/>
+        <f t="shared" si="55"/>
         <v>120.2</v>
       </c>
       <c r="W64" s="17">
-        <f t="shared" si="53"/>
+        <f t="shared" si="55"/>
         <v>93</v>
       </c>
       <c r="X64" s="17">
-        <f t="shared" ref="X64:Y64" si="54">X42+X44+X49+X51</f>
+        <f t="shared" ref="X64:Y64" si="56">X42+X44+X49+X51</f>
         <v>180.4</v>
       </c>
       <c r="Y64" s="17">
-        <f t="shared" si="54"/>
+        <f t="shared" si="56"/>
         <v>6.5000000000000009</v>
       </c>
       <c r="Z64" s="17">
@@ -4686,32 +5052,40 @@
       <c r="B65" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="M65" s="17">
+        <f t="shared" ref="M65:O65" si="57">M63-M64</f>
+        <v>48.5</v>
+      </c>
+      <c r="O65" s="17">
+        <f t="shared" si="57"/>
+        <v>-46.6</v>
+      </c>
       <c r="S65" s="17">
-        <f t="shared" ref="S65:T65" si="55">S63-S64</f>
+        <f t="shared" ref="S65:T65" si="58">S63-S64</f>
         <v>-58</v>
       </c>
       <c r="T65" s="17">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>-43.699999999999996</v>
       </c>
       <c r="U65" s="17">
-        <f t="shared" ref="U65:W65" si="56">U63-U64</f>
+        <f t="shared" ref="U65:W65" si="59">U63-U64</f>
         <v>-82.199999999999989</v>
       </c>
       <c r="V65" s="17">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>-92.9</v>
       </c>
       <c r="W65" s="17">
-        <f t="shared" si="56"/>
+        <f t="shared" si="59"/>
         <v>-80</v>
       </c>
       <c r="X65" s="17">
-        <f t="shared" ref="X65:Y65" si="57">X63-X64</f>
+        <f t="shared" ref="X65:Y65" si="60">X63-X64</f>
         <v>-56.2</v>
       </c>
       <c r="Y65" s="17">
-        <f t="shared" si="57"/>
+        <f t="shared" si="60"/>
         <v>61.3</v>
       </c>
       <c r="Z65" s="17">
@@ -4729,21 +5103,25 @@
       <c r="J67" s="40"/>
       <c r="L67" s="40"/>
       <c r="N67" s="40"/>
+      <c r="O67" s="29">
+        <f>O34/M34-1</f>
+        <v>6.0080645161290303E-2</v>
+      </c>
       <c r="P67" s="40"/>
       <c r="T67" s="29">
-        <f t="shared" ref="T67" si="58">T34/S34-1</f>
+        <f t="shared" ref="T67" si="61">T34/S34-1</f>
         <v>5.7602143335566014E-2</v>
       </c>
       <c r="U67" s="29">
-        <f t="shared" ref="U67" si="59">U34/T34-1</f>
+        <f t="shared" ref="U67" si="62">U34/T34-1</f>
         <v>0.21025965801139956</v>
       </c>
       <c r="V67" s="29">
-        <f t="shared" ref="V67:W67" si="60">V34/U34-1</f>
+        <f t="shared" ref="V67:W67" si="63">V34/U34-1</f>
         <v>2.3024594453165959E-2</v>
       </c>
       <c r="W67" s="29">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>-0.11150895140664963</v>
       </c>
       <c r="X67" s="29">
@@ -4777,7 +5155,13 @@
       <c r="H69" s="39"/>
       <c r="J69" s="39"/>
       <c r="L69" s="39"/>
+      <c r="M69" s="1">
+        <v>1.7208000000000001</v>
+      </c>
       <c r="N69" s="39"/>
+      <c r="O69" s="1">
+        <v>1.85</v>
+      </c>
       <c r="P69" s="39"/>
       <c r="S69" s="38">
         <v>3.0615000000000001</v>
@@ -4817,28 +5201,36 @@
       <c r="B70" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="M70" s="17">
+        <f t="shared" ref="M70" si="64">M69*M14</f>
+        <v>385.80336</v>
+      </c>
+      <c r="O70" s="17">
+        <f t="shared" ref="O70" si="65">O69*O14</f>
+        <v>419.76500000000004</v>
+      </c>
       <c r="S70" s="17">
-        <f t="shared" ref="S70:V70" si="61">S69*S14</f>
+        <f t="shared" ref="S70:V70" si="66">S69*S14</f>
         <v>604.34010000000001</v>
       </c>
       <c r="T70" s="17">
-        <f t="shared" si="61"/>
+        <f t="shared" si="66"/>
         <v>513.48154000000011</v>
       </c>
       <c r="U70" s="17">
-        <f t="shared" si="61"/>
+        <f t="shared" si="66"/>
         <v>509.62175999999994</v>
       </c>
       <c r="V70" s="17">
-        <f t="shared" si="61"/>
+        <f t="shared" si="66"/>
         <v>496.24181999999996</v>
       </c>
       <c r="W70" s="17">
-        <f t="shared" ref="W70:X70" si="62">W69*W14</f>
+        <f t="shared" ref="W70:X70" si="67">W69*W14</f>
         <v>338.46999999999997</v>
       </c>
       <c r="X70" s="17">
-        <f t="shared" si="62"/>
+        <f t="shared" si="67"/>
         <v>120.15685000000001</v>
       </c>
       <c r="Y70" s="17">
@@ -4854,20 +5246,28 @@
       <c r="B71" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="M71" s="17">
+        <f t="shared" ref="M71" si="68">M70-M65</f>
+        <v>337.30336</v>
+      </c>
+      <c r="O71" s="17">
+        <f t="shared" ref="O71" si="69">O70-O65</f>
+        <v>466.36500000000007</v>
+      </c>
       <c r="S71" s="17">
-        <f t="shared" ref="S71:V71" si="63">S70-S65</f>
+        <f t="shared" ref="S71:V71" si="70">S70-S65</f>
         <v>662.34010000000001</v>
       </c>
       <c r="T71" s="17">
-        <f t="shared" si="63"/>
+        <f t="shared" si="70"/>
         <v>557.18154000000015</v>
       </c>
       <c r="U71" s="17">
-        <f t="shared" si="63"/>
+        <f t="shared" si="70"/>
         <v>591.82175999999993</v>
       </c>
       <c r="V71" s="17">
-        <f t="shared" si="63"/>
+        <f t="shared" si="70"/>
         <v>589.14181999999994</v>
       </c>
       <c r="W71" s="17">
@@ -4895,32 +5295,41 @@
       <c r="B73" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="M73" s="41">
+        <f>M69/M61</f>
+        <v>0.69564255319148915</v>
+      </c>
+      <c r="N73" s="42"/>
+      <c r="O73" s="41">
+        <f>O69/O61</f>
+        <v>0.76237740646567365</v>
+      </c>
       <c r="S73" s="41">
-        <f t="shared" ref="S73:V73" si="64">S69/S61</f>
+        <f t="shared" ref="S73:V73" si="71">S69/S61</f>
         <v>1.6435683981506666</v>
       </c>
       <c r="T73" s="41">
-        <f t="shared" si="64"/>
+        <f t="shared" si="71"/>
         <v>1.2666046867291563</v>
       </c>
       <c r="U73" s="41">
-        <f t="shared" si="64"/>
+        <f t="shared" si="71"/>
         <v>1.2506055460122694</v>
       </c>
       <c r="V73" s="41">
-        <f t="shared" si="64"/>
+        <f t="shared" si="71"/>
         <v>1.1762072054989334</v>
       </c>
       <c r="W73" s="41">
-        <f t="shared" ref="W73:Y73" si="65">W69/W61</f>
+        <f t="shared" ref="W73:Y73" si="72">W69/W61</f>
         <v>0.82694844857073058</v>
       </c>
       <c r="X73" s="41">
-        <f t="shared" si="65"/>
+        <f t="shared" si="72"/>
         <v>0.32847689994532514</v>
       </c>
       <c r="Y73" s="41">
-        <f t="shared" si="65"/>
+        <f t="shared" si="72"/>
         <v>1.682962087123024</v>
       </c>
       <c r="Z73" s="41">
@@ -4930,7 +5339,7 @@
     </row>
     <row r="74" spans="1:35" s="41" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="71">
-        <f t="shared" ref="A74:A77" si="66">AVERAGE(S74:Z74)</f>
+        <f t="shared" ref="A74:A77" si="73">AVERAGE(S74:Z74)</f>
         <v>0.41374638068405767</v>
       </c>
       <c r="B74" s="41" t="s">
@@ -4944,31 +5353,31 @@
       <c r="N74" s="42"/>
       <c r="P74" s="42"/>
       <c r="S74" s="41">
-        <f t="shared" ref="S74:V74" si="67">S70/S4</f>
+        <f t="shared" ref="S74:V74" si="74">S70/S4</f>
         <v>0.58937009947337615</v>
       </c>
       <c r="T74" s="41">
-        <f t="shared" si="67"/>
+        <f t="shared" si="74"/>
         <v>0.50267404796867365</v>
       </c>
       <c r="U74" s="41">
-        <f t="shared" si="67"/>
+        <f t="shared" si="74"/>
         <v>0.46540799999999993</v>
       </c>
       <c r="V74" s="41">
-        <f t="shared" si="67"/>
+        <f t="shared" si="74"/>
         <v>0.43717894458638007</v>
       </c>
       <c r="W74" s="41">
-        <f t="shared" ref="W74:Y74" si="68">W70/W4</f>
+        <f t="shared" ref="W74:Y74" si="75">W70/W4</f>
         <v>0.29726857544352714</v>
       </c>
       <c r="X74" s="41">
-        <f t="shared" si="68"/>
+        <f t="shared" si="75"/>
         <v>0.10402289845035063</v>
       </c>
       <c r="Y74" s="41">
-        <f t="shared" si="68"/>
+        <f t="shared" si="75"/>
         <v>0.54410087440996679</v>
       </c>
       <c r="Z74" s="41">
@@ -4987,7 +5396,7 @@
     </row>
     <row r="75" spans="1:35" s="41" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="71">
-        <f t="shared" si="66"/>
+        <f t="shared" si="73"/>
         <v>0.45016822490598901</v>
       </c>
       <c r="B75" s="41" t="s">
@@ -5001,31 +5410,31 @@
       <c r="N75" s="42"/>
       <c r="P75" s="42"/>
       <c r="S75" s="41">
-        <f t="shared" ref="S75:V75" si="69">S71/S4</f>
+        <f t="shared" ref="S75:V75" si="76">S71/S4</f>
         <v>0.64593339184708398</v>
       </c>
       <c r="T75" s="41">
-        <f t="shared" si="69"/>
+        <f t="shared" si="76"/>
         <v>0.54545427312775341</v>
       </c>
       <c r="U75" s="41">
-        <f t="shared" si="69"/>
+        <f t="shared" si="76"/>
         <v>0.54047649315068491</v>
       </c>
       <c r="V75" s="41">
-        <f t="shared" si="69"/>
+        <f t="shared" si="76"/>
         <v>0.51902195401286233</v>
       </c>
       <c r="W75" s="41">
-        <f t="shared" ref="W75:Y75" si="70">W71/W4</f>
+        <f t="shared" ref="W75:Y75" si="77">W71/W4</f>
         <v>0.36753030036887407</v>
       </c>
       <c r="X75" s="41">
-        <f t="shared" si="70"/>
+        <f t="shared" si="77"/>
         <v>0.15267669465847114</v>
       </c>
       <c r="Y75" s="41">
-        <f t="shared" si="70"/>
+        <f t="shared" si="77"/>
         <v>0.49666606825040632</v>
       </c>
       <c r="Z75" s="41">
@@ -5044,7 +5453,7 @@
     </row>
     <row r="76" spans="1:35" s="41" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="71">
-        <f t="shared" si="66"/>
+        <f t="shared" si="73"/>
         <v>8.7576011619956287</v>
       </c>
       <c r="B76" s="41" t="s">
@@ -5058,31 +5467,31 @@
       <c r="N76" s="42"/>
       <c r="P76" s="42"/>
       <c r="S76" s="41">
-        <f t="shared" ref="S76:V76" si="71">S69/S13</f>
+        <f t="shared" ref="S76:V76" si="78">S69/S13</f>
         <v>9.184499999999991</v>
       </c>
       <c r="T76" s="41">
-        <f t="shared" si="71"/>
+        <f t="shared" si="78"/>
         <v>8.0863234645669291</v>
       </c>
       <c r="U76" s="41">
-        <f t="shared" si="71"/>
+        <f t="shared" si="78"/>
         <v>9.0358468085106303</v>
       </c>
       <c r="V76" s="41">
-        <f t="shared" si="71"/>
+        <f t="shared" si="78"/>
         <v>9.072062522851926</v>
       </c>
       <c r="W76" s="41">
-        <f t="shared" ref="W76:Y76" si="72">W69/W13</f>
+        <f t="shared" ref="W76:Y76" si="79">W69/W13</f>
         <v>8.0780429594272327</v>
       </c>
       <c r="X76" s="41">
-        <f t="shared" si="72"/>
+        <f t="shared" si="79"/>
         <v>6.8661057142857596</v>
       </c>
       <c r="Y76" s="41">
-        <f t="shared" si="72"/>
+        <f t="shared" si="79"/>
         <v>13.216946616541351</v>
       </c>
       <c r="Z76" s="41">
@@ -5101,7 +5510,7 @@
     </row>
     <row r="77" spans="1:35" s="41" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="71">
-        <f t="shared" si="66"/>
+        <f t="shared" si="73"/>
         <v>9.7642266095637211</v>
       </c>
       <c r="B77" s="41" t="s">
@@ -5115,31 +5524,31 @@
       <c r="N77" s="42"/>
       <c r="P77" s="42"/>
       <c r="S77" s="41">
-        <f t="shared" ref="S77:V77" si="73">S71/S12</f>
+        <f t="shared" ref="S77:V77" si="80">S71/S12</f>
         <v>10.06595896656534</v>
       </c>
       <c r="T77" s="41">
-        <f t="shared" si="73"/>
+        <f t="shared" si="80"/>
         <v>8.774512440944882</v>
       </c>
       <c r="U77" s="41">
-        <f t="shared" si="73"/>
+        <f t="shared" si="80"/>
         <v>10.493293617021266</v>
       </c>
       <c r="V77" s="41">
-        <f t="shared" si="73"/>
+        <f t="shared" si="80"/>
         <v>10.770417184643518</v>
       </c>
       <c r="W77" s="41">
-        <f t="shared" ref="W77:Y77" si="74">W71/W12</f>
+        <f t="shared" ref="W77:Y77" si="81">W71/W12</f>
         <v>9.9873508353222267</v>
       </c>
       <c r="X77" s="41">
-        <f t="shared" si="74"/>
+        <f t="shared" si="81"/>
         <v>10.077534285714352</v>
       </c>
       <c r="Y77" s="41">
-        <f t="shared" si="74"/>
+        <f t="shared" si="81"/>
         <v>12.064690977443609</v>
       </c>
       <c r="Z77" s="41">
@@ -5168,11 +5577,13 @@
     <hyperlink ref="X1" r:id="rId2" xr:uid="{92846B6F-2839-284E-AA85-90B408C1E203}"/>
     <hyperlink ref="V1" r:id="rId3" xr:uid="{13285A00-2106-4F98-B9F0-34A6A260A094}"/>
     <hyperlink ref="T1" r:id="rId4" xr:uid="{769CF0C5-F50D-4DA3-90F8-F8D13713771E}"/>
+    <hyperlink ref="O1" r:id="rId5" xr:uid="{269C442D-1224-4529-B6A0-B4A457C4FBF1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
   <ignoredErrors>
-    <ignoredError sqref="X9 AA7 AA11 AA9 AB11:AI11 AB9:AI9 AB7:AC7 AD7:AI7" formula="1"/>
+    <ignoredError sqref="X9 AA7 AA11 AA9 AB11:AI11 AB9:AI9 AB7:AC7 AD7:AI7 O7 M7 M11" formula="1"/>
   </ignoredErrors>
-  <drawing r:id="rId5"/>
+  <drawing r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>